<commit_message>
Add menu Import User Alumni
</commit_message>
<xml_diff>
--- a/storage/Template Import User Alumni.xlsx
+++ b/storage/Template Import User Alumni.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\tracer\storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB64C2FC-5960-47B5-813F-5D88BBD1907C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFD6CA1-8E58-46B0-8909-544EB2999938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-2370" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{25E3BB40-640E-44D8-A8BB-0A45A82EC1AB}"/>
+    <workbookView xWindow="20370" yWindow="-2370" windowWidth="29040" windowHeight="15720" xr2:uid="{25E3BB40-640E-44D8-A8BB-0A45A82EC1AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>D3 Farmasi</t>
   </si>
@@ -231,16 +231,108 @@
     <t>pilihan prodi yang tersdia pada aplikasi tracer sebagai berikut:</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <i/>
+    <t>nilai akan menjadi 0 jika diisi selain angka</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">kolom pertama: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>data tidak akan disimpan</t>
+      <t>nama</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kolom kedua:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nim</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">kolom ketiga: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>prodi</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kolom keempat:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> angkatan</t>
+    </r>
+  </si>
+  <si>
+    <t>*Data yang akan disimpan hanya pada sheet pertama (Sheet1)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">hanya menyimpan data bertipe angka/tahun (contoh </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2023</t>
     </r>
     <r>
       <rPr>
@@ -251,161 +343,85 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>nim1</t>
+  </si>
+  <si>
+    <t>nim2</t>
+  </si>
+  <si>
+    <t>nim3</t>
+  </si>
+  <si>
+    <t>nim4</t>
+  </si>
+  <si>
+    <t>nim5</t>
+  </si>
+  <si>
+    <t>S1 Gizi</t>
+  </si>
+  <si>
+    <t>D3 Ilmu Gizi</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>data bernilai sebagai</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 'tidak ditemukan'</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> jika format penulisan tidak sesuai</t>
     </r>
   </si>
   <si>
-    <t>nilai akan menjadi 0 jika diisi selain angka</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">kolom pertama: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>nama</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>kolom kedua:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> nim</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">kolom ketiga: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>prodi</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>kolom keempat:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> angkatan</t>
-    </r>
-  </si>
-  <si>
-    <t>*Data yang akan disimpan hanya pada sheet pertama (Sheet1)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">hanya menyimpan data bertipe angka/tahun (contoh </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2023</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>alunmni1</t>
-  </si>
-  <si>
-    <t>nim1</t>
-  </si>
-  <si>
-    <t>alunmni2</t>
-  </si>
-  <si>
-    <t>nim2</t>
-  </si>
-  <si>
-    <t>alunmni3</t>
-  </si>
-  <si>
-    <t>nim3</t>
-  </si>
-  <si>
-    <t>alunmni4</t>
-  </si>
-  <si>
-    <t>nim4</t>
-  </si>
-  <si>
-    <t>alunmni5</t>
-  </si>
-  <si>
-    <t>nim5</t>
+    <t>alumni1</t>
+  </si>
+  <si>
+    <t>alumni2</t>
+  </si>
+  <si>
+    <t>alumni3</t>
+  </si>
+  <si>
+    <t>alumni4</t>
+  </si>
+  <si>
+    <t>alumni5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -491,6 +507,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -852,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474205F8-1B75-4B58-A18A-CBD851E01D53}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,10 +886,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -877,10 +900,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -891,10 +914,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -905,13 +928,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="D4">
         <v>2004</v>
@@ -919,13 +942,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>2005</v>
@@ -942,30 +965,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE08366-BDFE-4F3B-A4DB-26D9E60BE20A}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66.85546875" customWidth="1"/>
     <col min="2" max="2" width="66" customWidth="1"/>
-    <col min="3" max="3" width="62.28515625" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" customWidth="1"/>
     <col min="4" max="4" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -979,7 +1002,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -993,7 +1016,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="3"/>
     </row>
@@ -1053,7 +1076,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G13" s="4"/>
     </row>
@@ -1065,7 +1088,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>